<commit_message>
Now it works for if 2 or more table comes with same mail
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet.altin\Documents\UiPath\HTML_to_DataTable\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOS\Renova\UiPath-Personal-Project\HTML_to_DataTable\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68266F30-D28F-47DA-9E67-E6A12A722251}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2BCE90-7B6D-4B63-A65D-3F048A4D3B19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,12 +29,6 @@
   </si>
   <si>
     <t>Paths</t>
-  </si>
-  <si>
-    <t>HTML.txt</t>
-  </si>
-  <si>
-    <t>Output.xlsx</t>
   </si>
   <si>
     <t>HTMLtxt_Path</t>
@@ -59,6 +53,12 @@
   </si>
   <si>
     <t>TABLO ÖRNEĞİ</t>
+  </si>
+  <si>
+    <t>Output/</t>
+  </si>
+  <si>
+    <t>Data/HTML.txt</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:D880"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -586,19 +586,19 @@
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D8" s="8"/>
     </row>
@@ -614,17 +614,17 @@
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="8"/>
     </row>
@@ -635,17 +635,17 @@
     <row r="14" spans="1:4" ht="14.25" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="8"/>
     </row>

</xml_diff>